<commit_message>
Preprocessing improved. Implementing first algos.
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophdrechsel/Documents/Personal/Uni/ML_Seminar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31AA156-20B6-374F-ABB0-97AAFF6CC071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF73AC52-73E0-0847-92DF-17619D01F349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E2508C16-089A-D04D-B8EE-8A05B3D2C7AB}"/>
   </bookViews>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B44F3D5-9A1F-B347-AB45-6DB5881AB1D0}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,10 +634,10 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -645,10 +645,10 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -656,10 +656,10 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -667,10 +667,10 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -678,10 +678,10 @@
         <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -689,10 +689,10 @@
         <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -700,10 +700,10 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -711,10 +711,10 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -722,10 +722,10 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -733,10 +733,10 @@
         <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -744,10 +744,10 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -755,10 +755,10 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -766,10 +766,10 @@
         <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -777,10 +777,10 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -788,10 +788,10 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -799,10 +799,10 @@
         <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -810,10 +810,10 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -821,10 +821,10 @@
         <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding feature selection via lasso.
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophdrechsel/Documents/Personal/Uni/ML_Seminar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56806E78-35A1-D146-A8A2-CD728B6AC80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11150858-3996-724B-8051-1313E8BDA999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E2508C16-089A-D04D-B8EE-8A05B3D2C7AB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>age</t>
   </si>
@@ -175,13 +175,7 @@
     <t>did r vote in 2012 election</t>
   </si>
   <si>
-    <t>remember if voted in 2016 election</t>
-  </si>
-  <si>
     <t>vote12</t>
-  </si>
-  <si>
-    <t>vote16</t>
   </si>
   <si>
     <t>natsoc</t>
@@ -572,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B44F3D5-9A1F-B347-AB45-6DB5881AB1D0}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,7 +770,7 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
@@ -787,10 +781,10 @@
         <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -798,10 +792,10 @@
         <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,10 +803,10 @@
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -820,10 +814,10 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -831,10 +825,10 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -842,10 +836,10 @@
         <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -853,10 +847,10 @@
         <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -864,42 +858,31 @@
         <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>